<commit_message>
modifications sur le canvas
</commit_message>
<xml_diff>
--- a/tools/fichier_excel/GroupeTD-GroupeProjet - ProjetInformatique.xlsx
+++ b/tools/fichier_excel/GroupeTD-GroupeProjet - ProjetInformatique.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29426"/>
   <workbookPr filterPrivacy="1" codeName="ThisWorkbook" autoCompressPictures="0"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF387343-2435-46C3-9F35-ED1C6D1CFB80}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{347F63C4-753C-4E79-B2FD-96B818BBD834}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" tabRatio="894" firstSheet="7" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="894" firstSheet="2" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1a-Identification Projet" sheetId="39" r:id="rId1"/>
@@ -185,7 +185,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="620" uniqueCount="345">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="647" uniqueCount="351">
   <si>
     <t>Responsable</t>
   </si>
@@ -994,22 +994,10 @@
     <t>Période du 03.11.2025 au 09.11.2024</t>
   </si>
   <si>
-    <t>Période du 10.11.2025 au 16.11.12025</t>
-  </si>
-  <si>
-    <t>Période du 17.11.12025 au 23.11.12025</t>
-  </si>
-  <si>
-    <t>Période du 24.11.12025 au 30.11.12025</t>
-  </si>
-  <si>
     <t>Période du 01.12.2025 au 07.12.2025</t>
   </si>
   <si>
     <t>Période du 08.12.2025 au 14.12.2025</t>
-  </si>
-  <si>
-    <t>Période du 15.12.2025 au 21.12.2025</t>
   </si>
   <si>
     <t>Gihalu Russel</t>
@@ -1187,12 +1175,6 @@
     <t>Lancer et Diriger une réunion tous les dimanches</t>
   </si>
   <si>
-    <t>In Progress</t>
-  </si>
-  <si>
-    <t>Faire les modifications  demandées par le proffesseur sur le CC2</t>
-  </si>
-  <si>
     <t>CC4(recette finale)</t>
   </si>
   <si>
@@ -1283,6 +1265,42 @@
   </si>
   <si>
     <t>L'équipe doit communiquer sur Whatsapp . (Voir action numéro 2)</t>
+  </si>
+  <si>
+    <t>Période du 24.11.2025 au 30.11.2025</t>
+  </si>
+  <si>
+    <t>Période du 10.11.2025 au 16.11.2025</t>
+  </si>
+  <si>
+    <t>Période du 17.11.2025 au 23.11.2025</t>
+  </si>
+  <si>
+    <t>1. Le responsable du projet était malade, ce qui a causé son absence à la présentation.</t>
+  </si>
+  <si>
+    <t>2. A cause des contrôles continues, on était obligé de décaler la date du début de la partie finale par rapport au planning initial</t>
+  </si>
+  <si>
+    <t>1. L'équipe s'est adaptée à l'absence du responsable pour gérer la présentation de la partie gestion</t>
+  </si>
+  <si>
+    <t>1. L'équipe a accéléré le travail pour finir plus tôt que le planning</t>
+  </si>
+  <si>
+    <t>2. L'équipe a fini le travail technique planifié</t>
+  </si>
+  <si>
+    <t>3. L'équipe a bien présenté la partie finale technique</t>
+  </si>
+  <si>
+    <t>Faire les modifications demandées par le professeur sur le CC2</t>
+  </si>
+  <si>
+    <t>Remplacer le responsable du groupe durant son indisponibilité</t>
+  </si>
+  <si>
+    <t>DD,DW</t>
   </si>
 </sst>
 </file>
@@ -7604,9 +7622,39 @@
     <xf numFmtId="14" fontId="4" fillId="80" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="68" borderId="46" xfId="956" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="68" borderId="34" xfId="956" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="68" borderId="45" xfId="956" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="71" borderId="47" xfId="292" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="71" borderId="0" xfId="292" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="71" borderId="49" xfId="292" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="71" borderId="48" xfId="292" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="71" borderId="21" xfId="292" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="14" fontId="5" fillId="71" borderId="50" xfId="292" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="21" fillId="72" borderId="2" xfId="956" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="73" borderId="2" xfId="956" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="73" borderId="2" xfId="956" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -7631,35 +7679,11 @@
     <xf numFmtId="0" fontId="7" fillId="73" borderId="2" xfId="956" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="68" borderId="46" xfId="956" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="68" borderId="34" xfId="956" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="68" borderId="45" xfId="956" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="71" borderId="47" xfId="292" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="71" borderId="0" xfId="292" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="71" borderId="49" xfId="292" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="14" fontId="4" fillId="71" borderId="48" xfId="292" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="71" borderId="21" xfId="292" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="14" fontId="5" fillId="71" borderId="50" xfId="292" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="73" borderId="2" xfId="956" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="96" fillId="69" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="96" fillId="69" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="68" borderId="46" xfId="958" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
@@ -7682,13 +7706,7 @@
     <xf numFmtId="0" fontId="95" fillId="69" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="96" fillId="69" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="19" fillId="69" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="96" fillId="69" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="68" borderId="46" xfId="957" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -7884,6 +7902,15 @@
     <xf numFmtId="0" fontId="8" fillId="71" borderId="21" xfId="946" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="100" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="100" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="100" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="68" borderId="56" xfId="957" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -7904,15 +7931,6 @@
     </xf>
     <xf numFmtId="0" fontId="101" fillId="78" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="100" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="100" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="100" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="69" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -8127,56 +8145,55 @@
     <cellStyle name="_Solution_Monitoring_Tools_File_V2_83090147-DDQ-TAV-EN-001_OUTILS_PILOTAGE-1" xfId="185" xr:uid="{00000000-0005-0000-0000-0000B8000000}"/>
     <cellStyle name="_Solution_Monitoring_Tools_File_V2_dossierpilotage_dts_2012_10_19" xfId="186" xr:uid="{00000000-0005-0000-0000-0000B9000000}"/>
     <cellStyle name="12Under" xfId="187" xr:uid="{00000000-0005-0000-0000-0000BA000000}"/>
-    <cellStyle name="20 % - Akzent1" xfId="194" builtinId="30" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent2" xfId="195" builtinId="34" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent3" xfId="196" builtinId="38" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent4" xfId="197" builtinId="42" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent5" xfId="198" builtinId="46" customBuiltin="1"/>
-    <cellStyle name="20 % - Akzent6" xfId="199" builtinId="50" customBuiltin="1"/>
     <cellStyle name="20 % - Accent1 2" xfId="188" xr:uid="{00000000-0005-0000-0000-0000BC000000}"/>
     <cellStyle name="20 % - Accent2 2" xfId="189" xr:uid="{00000000-0005-0000-0000-0000BE000000}"/>
     <cellStyle name="20 % - Accent3 2" xfId="190" xr:uid="{00000000-0005-0000-0000-0000C0000000}"/>
     <cellStyle name="20 % - Accent4 2" xfId="191" xr:uid="{00000000-0005-0000-0000-0000C2000000}"/>
     <cellStyle name="20 % - Accent5 2" xfId="192" xr:uid="{00000000-0005-0000-0000-0000C4000000}"/>
     <cellStyle name="20 % - Accent6 2" xfId="193" xr:uid="{00000000-0005-0000-0000-0000C6000000}"/>
-    <cellStyle name="40 % - Akzent1" xfId="206" builtinId="31" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent2" xfId="207" builtinId="35" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent3" xfId="208" builtinId="39" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent4" xfId="209" builtinId="43" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent5" xfId="210" builtinId="47" customBuiltin="1"/>
-    <cellStyle name="40 % - Akzent6" xfId="211" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="20% - Accent1" xfId="194" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="195" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="196" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="197" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="198" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="199" builtinId="50" customBuiltin="1"/>
     <cellStyle name="40 % - Accent1 2" xfId="200" xr:uid="{00000000-0005-0000-0000-0000CE000000}"/>
     <cellStyle name="40 % - Accent2 2" xfId="201" xr:uid="{00000000-0005-0000-0000-0000D0000000}"/>
     <cellStyle name="40 % - Accent3 2" xfId="202" xr:uid="{00000000-0005-0000-0000-0000D2000000}"/>
     <cellStyle name="40 % - Accent4 2" xfId="203" xr:uid="{00000000-0005-0000-0000-0000D4000000}"/>
     <cellStyle name="40 % - Accent5 2" xfId="204" xr:uid="{00000000-0005-0000-0000-0000D6000000}"/>
     <cellStyle name="40 % - Accent6 2" xfId="205" xr:uid="{00000000-0005-0000-0000-0000D8000000}"/>
-    <cellStyle name="60 % - Akzent1" xfId="218" builtinId="32" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent2" xfId="219" builtinId="36" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent3" xfId="220" builtinId="40" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent4" xfId="221" builtinId="44" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent5" xfId="222" builtinId="48" customBuiltin="1"/>
-    <cellStyle name="60 % - Akzent6" xfId="223" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="206" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="207" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="208" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="209" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="210" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="211" builtinId="51" customBuiltin="1"/>
     <cellStyle name="60 % - Accent1 2" xfId="212" xr:uid="{00000000-0005-0000-0000-0000E0000000}"/>
     <cellStyle name="60 % - Accent2 2" xfId="213" xr:uid="{00000000-0005-0000-0000-0000E2000000}"/>
     <cellStyle name="60 % - Accent3 2" xfId="214" xr:uid="{00000000-0005-0000-0000-0000E4000000}"/>
     <cellStyle name="60 % - Accent4 2" xfId="215" xr:uid="{00000000-0005-0000-0000-0000E6000000}"/>
     <cellStyle name="60 % - Accent5 2" xfId="216" xr:uid="{00000000-0005-0000-0000-0000E8000000}"/>
     <cellStyle name="60 % - Accent6 2" xfId="217" xr:uid="{00000000-0005-0000-0000-0000EA000000}"/>
+    <cellStyle name="60% - Accent1" xfId="218" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="219" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="220" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="221" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="222" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="223" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="224" builtinId="29" customBuiltin="1"/>
     <cellStyle name="Accent1 2" xfId="225" xr:uid="{00000000-0005-0000-0000-0000F2000000}"/>
+    <cellStyle name="Accent2" xfId="226" builtinId="33" customBuiltin="1"/>
     <cellStyle name="Accent2 2" xfId="227" xr:uid="{00000000-0005-0000-0000-0000F4000000}"/>
+    <cellStyle name="Accent3" xfId="228" builtinId="37" customBuiltin="1"/>
     <cellStyle name="Accent3 2" xfId="229" xr:uid="{00000000-0005-0000-0000-0000F6000000}"/>
+    <cellStyle name="Accent4" xfId="230" builtinId="41" customBuiltin="1"/>
     <cellStyle name="Accent4 2" xfId="231" xr:uid="{00000000-0005-0000-0000-0000F8000000}"/>
+    <cellStyle name="Accent5" xfId="232" builtinId="45" customBuiltin="1"/>
     <cellStyle name="Accent5 2" xfId="233" xr:uid="{00000000-0005-0000-0000-0000FA000000}"/>
+    <cellStyle name="Accent6" xfId="234" builtinId="49" customBuiltin="1"/>
     <cellStyle name="Accent6 2" xfId="235" xr:uid="{00000000-0005-0000-0000-0000FC000000}"/>
-    <cellStyle name="Akzent1" xfId="224" builtinId="29" customBuiltin="1"/>
-    <cellStyle name="Akzent2" xfId="226" builtinId="33" customBuiltin="1"/>
-    <cellStyle name="Akzent3" xfId="228" builtinId="37" customBuiltin="1"/>
-    <cellStyle name="Akzent4" xfId="230" builtinId="41" customBuiltin="1"/>
-    <cellStyle name="Akzent5" xfId="232" builtinId="45" customBuiltin="1"/>
-    <cellStyle name="Akzent6" xfId="234" builtinId="49" customBuiltin="1"/>
     <cellStyle name="Bad" xfId="883" xr:uid="{00000000-0005-0000-0000-0000FE000000}"/>
-    <cellStyle name="Berechnung" xfId="245" builtinId="22" customBuiltin="1"/>
     <cellStyle name="Bord: quadrillage" xfId="236" xr:uid="{00000000-0005-0000-0000-0000FF000000}"/>
     <cellStyle name="Bord: quadrillage gras" xfId="237" xr:uid="{00000000-0005-0000-0000-000000010000}"/>
     <cellStyle name="Bord: quadrillage gras 2" xfId="1170" xr:uid="{E6CC26DB-73E0-447F-AC06-EED4707DF3BB}"/>
@@ -8187,6 +8204,7 @@
     <cellStyle name="branche_1 - Fiche descriptive" xfId="242" xr:uid="{00000000-0005-0000-0000-000005010000}"/>
     <cellStyle name="Caché" xfId="243" xr:uid="{00000000-0005-0000-0000-000006010000}"/>
     <cellStyle name="Calcul 2" xfId="244" xr:uid="{00000000-0005-0000-0000-000008010000}"/>
+    <cellStyle name="Calculation" xfId="245" builtinId="22" customBuiltin="1"/>
     <cellStyle name="CARTOUCHE_THOM" xfId="246" xr:uid="{00000000-0005-0000-0000-00000A010000}"/>
     <cellStyle name="Check Cell" xfId="1165" xr:uid="{00000000-0005-0000-0000-00000C010000}"/>
     <cellStyle name="Comma [0]" xfId="247" xr:uid="{00000000-0005-0000-0000-00000D010000}"/>
@@ -8274,9 +8292,7 @@
     <cellStyle name="Donnée 4" xfId="322" xr:uid="{00000000-0005-0000-0000-00005C010000}"/>
     <cellStyle name="Donnée 5" xfId="323" xr:uid="{00000000-0005-0000-0000-00005D010000}"/>
     <cellStyle name="Donnée_1 - Fiche descriptive" xfId="324" xr:uid="{00000000-0005-0000-0000-00005E010000}"/>
-    <cellStyle name="Eingabe" xfId="882" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Entrée 2" xfId="325" xr:uid="{00000000-0005-0000-0000-000060010000}"/>
-    <cellStyle name="Ergebnis" xfId="1150" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Euro" xfId="326" xr:uid="{00000000-0005-0000-0000-000061010000}"/>
     <cellStyle name="Euro 2" xfId="327" xr:uid="{00000000-0005-0000-0000-000062010000}"/>
     <cellStyle name="Euro 2 2" xfId="328" xr:uid="{00000000-0005-0000-0000-000063010000}"/>
@@ -8965,6 +8981,7 @@
     <cellStyle name="Hyperlink 2" xfId="879" xr:uid="{00000000-0005-0000-0000-000090030000}"/>
     <cellStyle name="Hyperlink 2 2" xfId="880" xr:uid="{00000000-0005-0000-0000-000091030000}"/>
     <cellStyle name="Hyperlink_1 - Fiche descriptive" xfId="881" xr:uid="{00000000-0005-0000-0000-000092030000}"/>
+    <cellStyle name="Input" xfId="882" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Insatisfaisant 2" xfId="884" xr:uid="{00000000-0005-0000-0000-000095030000}"/>
     <cellStyle name="item" xfId="885" xr:uid="{00000000-0005-0000-0000-000096030000}"/>
     <cellStyle name="item 2" xfId="886" xr:uid="{00000000-0005-0000-0000-000097030000}"/>
@@ -8997,6 +9014,7 @@
     <cellStyle name="Lien hypertexte 6 2" xfId="1306" xr:uid="{3157CAE7-E5F3-4808-A259-1024D05AC903}"/>
     <cellStyle name="Lien_x0018_hypertexte" xfId="911" xr:uid="{00000000-0005-0000-0000-0000B0030000}"/>
     <cellStyle name="Lien_x0018_hypertexte 2" xfId="912" xr:uid="{00000000-0005-0000-0000-0000B1030000}"/>
+    <cellStyle name="Linked Cell" xfId="913" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Masqué" xfId="914" xr:uid="{00000000-0005-0000-0000-0000B3030000}"/>
     <cellStyle name="Masqué 2" xfId="915" xr:uid="{00000000-0005-0000-0000-0000B4030000}"/>
     <cellStyle name="Masqué 2 2" xfId="916" xr:uid="{00000000-0005-0000-0000-0000B5030000}"/>
@@ -9029,6 +9047,7 @@
     <cellStyle name="Non modifiable 3" xfId="943" xr:uid="{00000000-0005-0000-0000-0000D1030000}"/>
     <cellStyle name="Non modifiable 3 2" xfId="944" xr:uid="{00000000-0005-0000-0000-0000D2030000}"/>
     <cellStyle name="Non modifiable 4" xfId="945" xr:uid="{00000000-0005-0000-0000-0000D3030000}"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="946" xr:uid="{00000000-0005-0000-0000-0000D5030000}"/>
     <cellStyle name="Normal 2 2" xfId="947" xr:uid="{00000000-0005-0000-0000-0000D6030000}"/>
     <cellStyle name="Normal 2 2 2" xfId="948" xr:uid="{00000000-0005-0000-0000-0000D7030000}"/>
@@ -9051,7 +9070,7 @@
     <cellStyle name="Normal_Maquette_TDB4 2" xfId="959" xr:uid="{00000000-0005-0000-0000-0000E2030000}"/>
     <cellStyle name="Normal_Project reporting template-87201044-MGPR-GRP-EN- 2" xfId="960" xr:uid="{00000000-0005-0000-0000-0000E3030000}"/>
     <cellStyle name="Normal_Solution_Monitoring_Dashboard_File 2" xfId="961" xr:uid="{00000000-0005-0000-0000-0000E4030000}"/>
-    <cellStyle name="Notiz" xfId="962" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Note" xfId="962" builtinId="10" customBuiltin="1"/>
     <cellStyle name="obsolete" xfId="963" xr:uid="{00000000-0005-0000-0000-0000E5030000}"/>
     <cellStyle name="one" xfId="964" xr:uid="{00000000-0005-0000-0000-0000E6030000}"/>
     <cellStyle name="Output" xfId="1113" xr:uid="{00000000-0005-0000-0000-0000E7030000}"/>
@@ -9207,7 +9226,6 @@
     <cellStyle name="SAPBEXundefined_1 - Fiche descriptive" xfId="1110" xr:uid="{00000000-0005-0000-0000-00007A040000}"/>
     <cellStyle name="Satisfaisant 2" xfId="1112" xr:uid="{00000000-0005-0000-0000-00007C040000}"/>
     <cellStyle name="Sortie 2" xfId="1114" xr:uid="{00000000-0005-0000-0000-00007E040000}"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
     <cellStyle name="StationEach" xfId="1115" xr:uid="{00000000-0005-0000-0000-00007F040000}"/>
     <cellStyle name="StationTot" xfId="1116" xr:uid="{00000000-0005-0000-0000-000080040000}"/>
     <cellStyle name="Style 1" xfId="1117" xr:uid="{00000000-0005-0000-0000-000081040000}"/>
@@ -9240,6 +9258,7 @@
     <cellStyle name="TitreSérie 4" xfId="1147" xr:uid="{00000000-0005-0000-0000-0000A0040000}"/>
     <cellStyle name="TitreSérie 5" xfId="1148" xr:uid="{00000000-0005-0000-0000-0000A1040000}"/>
     <cellStyle name="TitreSérie_1 - Fiche descriptive" xfId="1149" xr:uid="{00000000-0005-0000-0000-0000A2040000}"/>
+    <cellStyle name="Total" xfId="1150" builtinId="25" customBuiltin="1"/>
     <cellStyle name="TypeDonnée" xfId="1151" xr:uid="{00000000-0005-0000-0000-0000A4040000}"/>
     <cellStyle name="TypeDonnée 2" xfId="1152" xr:uid="{00000000-0005-0000-0000-0000A5040000}"/>
     <cellStyle name="TypeDonnée 2 2" xfId="1153" xr:uid="{00000000-0005-0000-0000-0000A6040000}"/>
@@ -9255,8 +9274,7 @@
     <cellStyle name="Variation 4" xfId="1163" xr:uid="{00000000-0005-0000-0000-0000B0040000}"/>
     <cellStyle name="Variation_1 - Fiche descriptive" xfId="1164" xr:uid="{00000000-0005-0000-0000-0000B1040000}"/>
     <cellStyle name="Vérification 2" xfId="1166" xr:uid="{00000000-0005-0000-0000-0000B3040000}"/>
-    <cellStyle name="Verknüpfte Zelle" xfId="913" builtinId="24" customBuiltin="1"/>
-    <cellStyle name="Warnender Text" xfId="1167" builtinId="11" customBuiltin="1"/>
+    <cellStyle name="Warning Text" xfId="1167" builtinId="11" customBuiltin="1"/>
     <cellStyle name="Обычный_2.1 GANTT" xfId="1168" xr:uid="{00000000-0005-0000-0000-0000B5040000}"/>
     <cellStyle name="標準_Application List with Client Dependencies DSL" xfId="1169" xr:uid="{00000000-0005-0000-0000-0000B6040000}"/>
   </cellStyles>
@@ -24761,7 +24779,7 @@
       <selection activeCell="Q9" sqref="Q9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.2"/>
   <cols>
     <col min="1" max="1" width="1.6640625" style="5" customWidth="1"/>
     <col min="2" max="2" width="11.44140625" style="5"/>
@@ -24783,11 +24801,11 @@
       <c r="I1" s="113"/>
       <c r="J1" s="113"/>
       <c r="K1" s="113"/>
-      <c r="L1" s="215" t="s">
+      <c r="L1" s="206" t="s">
         <v>27</v>
       </c>
-      <c r="M1" s="216"/>
-      <c r="N1" s="217"/>
+      <c r="M1" s="207"/>
+      <c r="N1" s="208"/>
       <c r="P1" s="24"/>
     </row>
     <row r="2" spans="2:16" ht="12.75" customHeight="1">
@@ -24801,11 +24819,11 @@
       <c r="I2" s="115"/>
       <c r="J2" s="115"/>
       <c r="K2" s="115"/>
-      <c r="L2" s="218">
+      <c r="L2" s="209">
         <v>45912</v>
       </c>
-      <c r="M2" s="219"/>
-      <c r="N2" s="220"/>
+      <c r="M2" s="210"/>
+      <c r="N2" s="211"/>
     </row>
     <row r="3" spans="2:16" ht="12.75" customHeight="1" thickBot="1">
       <c r="B3" s="116"/>
@@ -24818,34 +24836,34 @@
       <c r="I3" s="117"/>
       <c r="J3" s="117"/>
       <c r="K3" s="117"/>
-      <c r="L3" s="221" t="s">
+      <c r="L3" s="212" t="s">
         <v>28</v>
       </c>
-      <c r="M3" s="222"/>
-      <c r="N3" s="223"/>
+      <c r="M3" s="213"/>
+      <c r="N3" s="214"/>
       <c r="P3" s="24"/>
     </row>
     <row r="4" spans="2:16" ht="12.75" customHeight="1" thickBot="1">
       <c r="P4" s="25"/>
     </row>
     <row r="5" spans="2:16" ht="23.4" thickBot="1">
-      <c r="B5" s="206" t="s">
+      <c r="B5" s="215" t="s">
         <v>17</v>
       </c>
-      <c r="C5" s="206"/>
+      <c r="C5" s="215"/>
       <c r="D5" s="6"/>
-      <c r="E5" s="224" t="s">
-        <v>264</v>
-      </c>
-      <c r="F5" s="224"/>
-      <c r="G5" s="224"/>
-      <c r="H5" s="224"/>
-      <c r="I5" s="224"/>
-      <c r="J5" s="224"/>
-      <c r="K5" s="224"/>
-      <c r="L5" s="224"/>
-      <c r="M5" s="224"/>
-      <c r="N5" s="224"/>
+      <c r="E5" s="216" t="s">
+        <v>260</v>
+      </c>
+      <c r="F5" s="216"/>
+      <c r="G5" s="216"/>
+      <c r="H5" s="216"/>
+      <c r="I5" s="216"/>
+      <c r="J5" s="216"/>
+      <c r="K5" s="216"/>
+      <c r="L5" s="216"/>
+      <c r="M5" s="216"/>
+      <c r="N5" s="216"/>
     </row>
     <row r="6" spans="2:16" ht="12" customHeight="1" thickBot="1">
       <c r="B6" s="7"/>
@@ -24862,23 +24880,23 @@
       <c r="N6" s="9"/>
     </row>
     <row r="7" spans="2:16" ht="18" thickBot="1">
-      <c r="B7" s="206" t="s">
+      <c r="B7" s="215" t="s">
         <v>79</v>
       </c>
-      <c r="C7" s="206"/>
+      <c r="C7" s="215"/>
       <c r="D7" s="6"/>
-      <c r="E7" s="209" t="s">
-        <v>263</v>
-      </c>
-      <c r="F7" s="210"/>
-      <c r="G7" s="210"/>
-      <c r="H7" s="210"/>
-      <c r="I7" s="210"/>
-      <c r="J7" s="210"/>
-      <c r="K7" s="210"/>
-      <c r="L7" s="210"/>
-      <c r="M7" s="210"/>
-      <c r="N7" s="211"/>
+      <c r="E7" s="219" t="s">
+        <v>259</v>
+      </c>
+      <c r="F7" s="220"/>
+      <c r="G7" s="220"/>
+      <c r="H7" s="220"/>
+      <c r="I7" s="220"/>
+      <c r="J7" s="220"/>
+      <c r="K7" s="220"/>
+      <c r="L7" s="220"/>
+      <c r="M7" s="220"/>
+      <c r="N7" s="221"/>
     </row>
     <row r="8" spans="2:16" ht="9.6" customHeight="1" thickBot="1">
       <c r="B8" s="10"/>
@@ -24896,23 +24914,23 @@
       <c r="N8" s="12"/>
     </row>
     <row r="9" spans="2:16" ht="54.6" customHeight="1" thickBot="1">
-      <c r="B9" s="212" t="s">
+      <c r="B9" s="222" t="s">
         <v>2</v>
       </c>
-      <c r="C9" s="212"/>
+      <c r="C9" s="222"/>
       <c r="D9" s="6"/>
-      <c r="E9" s="213" t="s">
-        <v>277</v>
-      </c>
-      <c r="F9" s="214"/>
-      <c r="G9" s="214"/>
-      <c r="H9" s="214"/>
-      <c r="I9" s="214"/>
-      <c r="J9" s="214"/>
-      <c r="K9" s="214"/>
-      <c r="L9" s="214"/>
-      <c r="M9" s="214"/>
-      <c r="N9" s="214"/>
+      <c r="E9" s="223" t="s">
+        <v>273</v>
+      </c>
+      <c r="F9" s="224"/>
+      <c r="G9" s="224"/>
+      <c r="H9" s="224"/>
+      <c r="I9" s="224"/>
+      <c r="J9" s="224"/>
+      <c r="K9" s="224"/>
+      <c r="L9" s="224"/>
+      <c r="M9" s="224"/>
+      <c r="N9" s="224"/>
     </row>
     <row r="10" spans="2:16" ht="10.95" customHeight="1" thickBot="1">
       <c r="B10" s="10"/>
@@ -24930,23 +24948,23 @@
       <c r="N10" s="12"/>
     </row>
     <row r="11" spans="2:16" ht="61.2" customHeight="1" thickBot="1">
-      <c r="B11" s="206" t="s">
+      <c r="B11" s="215" t="s">
         <v>16</v>
       </c>
-      <c r="C11" s="206"/>
+      <c r="C11" s="215"/>
       <c r="D11" s="6"/>
-      <c r="E11" s="213" t="s">
+      <c r="E11" s="223" t="s">
         <v>67</v>
       </c>
-      <c r="F11" s="214"/>
-      <c r="G11" s="214"/>
-      <c r="H11" s="214"/>
-      <c r="I11" s="214"/>
-      <c r="J11" s="214"/>
-      <c r="K11" s="214"/>
-      <c r="L11" s="214"/>
-      <c r="M11" s="214"/>
-      <c r="N11" s="214"/>
+      <c r="F11" s="224"/>
+      <c r="G11" s="224"/>
+      <c r="H11" s="224"/>
+      <c r="I11" s="224"/>
+      <c r="J11" s="224"/>
+      <c r="K11" s="224"/>
+      <c r="L11" s="224"/>
+      <c r="M11" s="224"/>
+      <c r="N11" s="224"/>
     </row>
     <row r="12" spans="2:16" ht="10.95" customHeight="1" thickBot="1">
       <c r="B12" s="10"/>
@@ -24964,23 +24982,23 @@
       <c r="N12" s="12"/>
     </row>
     <row r="13" spans="2:16" ht="99" customHeight="1" thickBot="1">
-      <c r="B13" s="206" t="s">
+      <c r="B13" s="215" t="s">
         <v>3</v>
       </c>
-      <c r="C13" s="206"/>
+      <c r="C13" s="215"/>
       <c r="D13" s="6"/>
-      <c r="E13" s="207" t="s">
-        <v>265</v>
-      </c>
-      <c r="F13" s="208"/>
-      <c r="G13" s="208"/>
-      <c r="H13" s="208"/>
-      <c r="I13" s="208"/>
-      <c r="J13" s="208"/>
-      <c r="K13" s="208"/>
-      <c r="L13" s="208"/>
-      <c r="M13" s="208"/>
-      <c r="N13" s="208"/>
+      <c r="E13" s="217" t="s">
+        <v>261</v>
+      </c>
+      <c r="F13" s="218"/>
+      <c r="G13" s="218"/>
+      <c r="H13" s="218"/>
+      <c r="I13" s="218"/>
+      <c r="J13" s="218"/>
+      <c r="K13" s="218"/>
+      <c r="L13" s="218"/>
+      <c r="M13" s="218"/>
+      <c r="N13" s="218"/>
     </row>
     <row r="14" spans="2:16" ht="73.5" customHeight="1">
       <c r="B14" s="13"/>
@@ -25004,11 +25022,6 @@
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
   <mergeCells count="13">
-    <mergeCell ref="L1:N1"/>
-    <mergeCell ref="L2:N2"/>
-    <mergeCell ref="L3:N3"/>
-    <mergeCell ref="B5:C5"/>
-    <mergeCell ref="E5:N5"/>
     <mergeCell ref="B13:C13"/>
     <mergeCell ref="E13:N13"/>
     <mergeCell ref="B7:C7"/>
@@ -25017,6 +25030,11 @@
     <mergeCell ref="E9:N9"/>
     <mergeCell ref="B11:C11"/>
     <mergeCell ref="E11:N11"/>
+    <mergeCell ref="L1:N1"/>
+    <mergeCell ref="L2:N2"/>
+    <mergeCell ref="L3:N3"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="E5:N5"/>
   </mergeCells>
   <dataValidations count="1">
     <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E8:N8 E10:N10 E12:N12" xr:uid="{00000000-0002-0000-0000-000000000000}">
@@ -25038,11 +25056,11 @@
   </sheetPr>
   <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7:F7"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection sqref="A1:I3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.2"/>
   <cols>
     <col min="1" max="1" width="16" style="3" customWidth="1"/>
     <col min="2" max="2" width="52" style="3" customWidth="1"/>
@@ -25058,9 +25076,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="13.5" customHeight="1">
-      <c r="A1" s="271" t="str">
+      <c r="A1" s="271" t="e">
         <f>"LISTE DES DECISIONS au "&amp;TEXT(J2,"jj/mm/aaaa")</f>
-        <v>LISTE DES DECISIONS au 25/00/Freitag</v>
+        <v>#VALUE!</v>
       </c>
       <c r="B1" s="258"/>
       <c r="C1" s="258"/>
@@ -25070,11 +25088,11 @@
       <c r="G1" s="258"/>
       <c r="H1" s="258"/>
       <c r="I1" s="259"/>
-      <c r="J1" s="225" t="str">
+      <c r="J1" s="227" t="str">
         <f>'1a-Identification Projet'!$L1</f>
         <v>reference Tableau de bord</v>
       </c>
-      <c r="K1" s="226"/>
+      <c r="K1" s="228"/>
     </row>
     <row r="2" spans="1:11" ht="12.75" customHeight="1">
       <c r="A2" s="261"/>
@@ -25086,11 +25104,11 @@
       <c r="G2" s="261"/>
       <c r="H2" s="261"/>
       <c r="I2" s="262"/>
-      <c r="J2" s="227">
+      <c r="J2" s="229">
         <f>'1a-Identification Projet'!$L2</f>
         <v>45912</v>
       </c>
-      <c r="K2" s="228"/>
+      <c r="K2" s="230"/>
     </row>
     <row r="3" spans="1:11" ht="16.5" customHeight="1" thickBot="1">
       <c r="A3" s="264"/>
@@ -25102,11 +25120,11 @@
       <c r="G3" s="264"/>
       <c r="H3" s="264"/>
       <c r="I3" s="265"/>
-      <c r="J3" s="229" t="str">
+      <c r="J3" s="231" t="str">
         <f>'1a-Identification Projet'!$L3</f>
         <v>Organisation</v>
       </c>
-      <c r="K3" s="230"/>
+      <c r="K3" s="232"/>
     </row>
     <row r="4" spans="1:11" ht="12.75" customHeight="1" thickBot="1">
       <c r="A4" s="26"/>
@@ -25146,14 +25164,14 @@
         <v>1</v>
       </c>
       <c r="B6" s="266" t="s">
-        <v>342</v>
+        <v>336</v>
       </c>
       <c r="C6" s="266"/>
       <c r="D6" s="266"/>
       <c r="E6" s="266"/>
       <c r="F6" s="266"/>
       <c r="G6" s="91" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="H6" s="173">
         <v>45908</v>
@@ -25162,25 +25180,25 @@
         <v>46003</v>
       </c>
       <c r="J6" s="92" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="K6" s="93" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="30">
+    <row r="7" spans="1:11" ht="45">
       <c r="A7" s="90">
         <v>2</v>
       </c>
       <c r="B7" s="266" t="s">
-        <v>344</v>
+        <v>338</v>
       </c>
       <c r="C7" s="266"/>
       <c r="D7" s="266"/>
       <c r="E7" s="266"/>
       <c r="F7" s="266"/>
       <c r="G7" s="91" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="H7" s="173">
         <v>45910</v>
@@ -25189,7 +25207,7 @@
         <v>46003</v>
       </c>
       <c r="J7" s="92" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="K7" s="93" t="s">
         <v>22</v>
@@ -25200,14 +25218,14 @@
         <v>3</v>
       </c>
       <c r="B8" s="266" t="s">
-        <v>343</v>
+        <v>337</v>
       </c>
       <c r="C8" s="266"/>
       <c r="D8" s="266"/>
       <c r="E8" s="266"/>
       <c r="F8" s="266"/>
       <c r="G8" s="91" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="H8" s="173">
         <v>45936</v>
@@ -25216,7 +25234,7 @@
         <v>46003</v>
       </c>
       <c r="J8" s="92" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="K8" s="93" t="s">
         <v>22</v>
@@ -25291,11 +25309,11 @@
   </sheetPr>
   <dimension ref="A1:J31"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D36" sqref="D36"/>
+    <sheetView showGridLines="0" topLeftCell="B1" zoomScale="129" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="I2" sqref="I2:J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="13.2" outlineLevelRow="2"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.2" outlineLevelRow="2"/>
   <cols>
     <col min="1" max="1" width="33.6640625" style="3" customWidth="1"/>
     <col min="2" max="2" width="38.6640625" style="3" customWidth="1"/>
@@ -25323,11 +25341,11 @@
       <c r="F1" s="271"/>
       <c r="G1" s="271"/>
       <c r="H1" s="272"/>
-      <c r="I1" s="225" t="str">
+      <c r="I1" s="227" t="str">
         <f>'1a-Identification Projet'!$L1</f>
         <v>reference Tableau de bord</v>
       </c>
-      <c r="J1" s="226"/>
+      <c r="J1" s="228"/>
     </row>
     <row r="2" spans="1:10" ht="12.75" customHeight="1">
       <c r="A2" s="273"/>
@@ -25338,11 +25356,11 @@
       <c r="F2" s="274"/>
       <c r="G2" s="274"/>
       <c r="H2" s="275"/>
-      <c r="I2" s="227">
+      <c r="I2" s="229">
         <f>'1a-Identification Projet'!$L2</f>
         <v>45912</v>
       </c>
-      <c r="J2" s="228"/>
+      <c r="J2" s="230"/>
     </row>
     <row r="3" spans="1:10" ht="16.5" customHeight="1" thickBot="1">
       <c r="A3" s="276"/>
@@ -25353,11 +25371,11 @@
       <c r="F3" s="277"/>
       <c r="G3" s="277"/>
       <c r="H3" s="278"/>
-      <c r="I3" s="229" t="str">
+      <c r="I3" s="231" t="str">
         <f>'1a-Identification Projet'!$L3</f>
         <v>Organisation</v>
       </c>
-      <c r="J3" s="230"/>
+      <c r="J3" s="232"/>
     </row>
     <row r="4" spans="1:10" ht="13.8" thickBot="1">
       <c r="A4" s="41"/>
@@ -25433,7 +25451,7 @@
     </row>
     <row r="8" spans="1:10" ht="13.8" outlineLevel="1" thickBot="1">
       <c r="A8" s="59" t="s">
-        <v>330</v>
+        <v>324</v>
       </c>
       <c r="B8" s="59"/>
       <c r="C8" s="59"/>
@@ -25465,12 +25483,12 @@
     </row>
     <row r="10" spans="1:10" outlineLevel="1">
       <c r="A10" s="59" t="s">
-        <v>331</v>
+        <v>325</v>
       </c>
       <c r="B10" s="59"/>
       <c r="C10" s="59"/>
       <c r="D10" s="59" t="s">
-        <v>332</v>
+        <v>326</v>
       </c>
       <c r="E10" s="59"/>
       <c r="F10" s="59"/>
@@ -25483,12 +25501,12 @@
     </row>
     <row r="11" spans="1:10" ht="13.8" outlineLevel="2" thickBot="1">
       <c r="A11" s="59" t="s">
-        <v>333</v>
+        <v>327</v>
       </c>
       <c r="B11" s="59"/>
       <c r="C11" s="59"/>
       <c r="D11" s="59" t="s">
-        <v>334</v>
+        <v>328</v>
       </c>
       <c r="E11" s="59"/>
       <c r="F11" s="59"/>
@@ -25529,7 +25547,7 @@
     </row>
     <row r="14" spans="1:10" outlineLevel="1">
       <c r="A14" s="59" t="s">
-        <v>335</v>
+        <v>329</v>
       </c>
       <c r="B14" s="59"/>
       <c r="C14" s="59"/>
@@ -25549,7 +25567,7 @@
     </row>
     <row r="15" spans="1:10" outlineLevel="2">
       <c r="A15" s="59" t="s">
-        <v>336</v>
+        <v>330</v>
       </c>
       <c r="B15" s="59"/>
       <c r="C15" s="59"/>
@@ -25569,7 +25587,7 @@
     </row>
     <row r="16" spans="1:10" outlineLevel="2">
       <c r="A16" s="59" t="s">
-        <v>327</v>
+        <v>321</v>
       </c>
       <c r="B16" s="59"/>
       <c r="C16" s="59"/>
@@ -25589,7 +25607,7 @@
     </row>
     <row r="17" spans="1:10" ht="13.8" outlineLevel="2" thickBot="1">
       <c r="A17" s="59" t="s">
-        <v>337</v>
+        <v>331</v>
       </c>
       <c r="B17" s="59"/>
       <c r="C17" s="59"/>
@@ -25623,7 +25641,7 @@
     </row>
     <row r="19" spans="1:10" outlineLevel="1">
       <c r="A19" s="59" t="s">
-        <v>338</v>
+        <v>332</v>
       </c>
       <c r="B19" s="59"/>
       <c r="C19" s="59"/>
@@ -25884,11 +25902,11 @@
   </sheetPr>
   <dimension ref="A1:L15"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView showGridLines="0" topLeftCell="A3" zoomScale="126" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="D26" sqref="D26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="13.2" outlineLevelRow="2"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.2" outlineLevelRow="2"/>
   <cols>
     <col min="1" max="1" width="32.5546875" style="3" customWidth="1"/>
     <col min="2" max="2" width="76.33203125" style="3" customWidth="1"/>
@@ -25906,31 +25924,31 @@
       </c>
       <c r="B1" s="280"/>
       <c r="C1" s="280"/>
-      <c r="D1" s="225" t="str">
+      <c r="D1" s="227" t="str">
         <f>'1a-Identification Projet'!$L1</f>
         <v>reference Tableau de bord</v>
       </c>
-      <c r="E1" s="226"/>
+      <c r="E1" s="228"/>
     </row>
     <row r="2" spans="1:12" ht="12.75" customHeight="1">
       <c r="A2" s="281"/>
       <c r="B2" s="282"/>
       <c r="C2" s="282"/>
-      <c r="D2" s="227">
+      <c r="D2" s="229">
         <f>'1a-Identification Projet'!$L2</f>
         <v>45912</v>
       </c>
-      <c r="E2" s="228"/>
+      <c r="E2" s="230"/>
     </row>
     <row r="3" spans="1:12" ht="16.5" customHeight="1" thickBot="1">
       <c r="A3" s="283"/>
       <c r="B3" s="284"/>
       <c r="C3" s="284"/>
-      <c r="D3" s="229" t="str">
+      <c r="D3" s="231" t="str">
         <f>'1a-Identification Projet'!$L3</f>
         <v>Organisation</v>
       </c>
-      <c r="E3" s="230"/>
+      <c r="E3" s="232"/>
     </row>
     <row r="4" spans="1:12" ht="12.75" customHeight="1" thickBot="1">
       <c r="B4" s="26"/>
@@ -25963,10 +25981,10 @@
     </row>
     <row r="7" spans="1:12">
       <c r="A7" s="59" t="s">
-        <v>324</v>
+        <v>318</v>
       </c>
       <c r="B7" s="59" t="s">
-        <v>323</v>
+        <v>317</v>
       </c>
       <c r="C7" s="59">
         <v>45926</v>
@@ -25980,10 +25998,10 @@
     </row>
     <row r="8" spans="1:12" outlineLevel="2">
       <c r="A8" s="59" t="s">
-        <v>325</v>
+        <v>319</v>
       </c>
       <c r="B8" s="59" t="s">
-        <v>326</v>
+        <v>320</v>
       </c>
       <c r="C8" s="59">
         <v>45937</v>
@@ -25997,10 +26015,10 @@
     </row>
     <row r="9" spans="1:12" outlineLevel="2">
       <c r="A9" s="59" t="s">
-        <v>327</v>
+        <v>321</v>
       </c>
       <c r="B9" s="59" t="s">
-        <v>328</v>
+        <v>322</v>
       </c>
       <c r="C9" s="59">
         <v>45948</v>
@@ -26021,10 +26039,10 @@
     </row>
     <row r="10" spans="1:12" s="4" customFormat="1" outlineLevel="2">
       <c r="A10" s="59" t="s">
-        <v>322</v>
+        <v>316</v>
       </c>
       <c r="B10" s="59" t="s">
-        <v>329</v>
+        <v>323</v>
       </c>
       <c r="C10" s="59">
         <v>46003</v>
@@ -26094,11 +26112,11 @@
   </sheetPr>
   <dimension ref="A1:I22"/>
   <sheetViews>
-    <sheetView showGridLines="0" showZeros="0" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView showGridLines="0" showZeros="0" topLeftCell="A6" zoomScale="89" zoomScaleNormal="80" workbookViewId="0">
+      <selection sqref="A1:E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.2"/>
   <cols>
     <col min="1" max="1" width="71.77734375" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="105.21875" style="3" bestFit="1" customWidth="1"/>
@@ -26200,14 +26218,14 @@
     </row>
     <row r="7" spans="1:9" ht="26.4">
       <c r="A7" s="60" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="B7" s="62" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="C7" s="63"/>
       <c r="D7" s="64" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="E7" s="63"/>
       <c r="F7" s="65"/>
@@ -26215,16 +26233,16 @@
       <c r="H7" s="65"/>
       <c r="I7" s="66"/>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" ht="26.4">
       <c r="A8" s="60" t="s">
-        <v>302</v>
+        <v>298</v>
       </c>
       <c r="B8" s="62" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="C8" s="63"/>
       <c r="D8" s="64" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="E8" s="63"/>
       <c r="F8" s="65"/>
@@ -26234,14 +26252,14 @@
     </row>
     <row r="9" spans="1:9">
       <c r="A9" s="61" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="B9" s="62" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="C9" s="63"/>
       <c r="D9" s="64" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="E9" s="63"/>
       <c r="F9" s="65"/>
@@ -26334,14 +26352,14 @@
     </row>
     <row r="16" spans="1:9">
       <c r="A16" s="71" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="B16" s="72" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="C16" s="63"/>
       <c r="D16" s="64" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="E16" s="63"/>
       <c r="F16" s="65"/>
@@ -26351,14 +26369,14 @@
     </row>
     <row r="17" spans="1:9" ht="21" customHeight="1">
       <c r="A17" s="71" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="B17" s="72" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="C17" s="63"/>
       <c r="D17" s="64" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="E17" s="63"/>
       <c r="F17" s="65"/>
@@ -26368,14 +26386,14 @@
     </row>
     <row r="18" spans="1:9" ht="26.4">
       <c r="A18" s="74" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="B18" s="72" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="C18" s="63"/>
       <c r="D18" s="64" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="E18" s="63"/>
       <c r="F18" s="65"/>
@@ -26456,11 +26474,11 @@
   </sheetPr>
   <dimension ref="A1:AM209"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="B17" zoomScale="76" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="N29" sqref="N29"/>
+    <sheetView showGridLines="0" topLeftCell="C20" zoomScale="112" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="Q30" sqref="Q30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.2"/>
   <cols>
     <col min="1" max="1" width="1.6640625" style="3" customWidth="1"/>
     <col min="2" max="2" width="14" style="3" customWidth="1"/>
@@ -26487,14 +26505,14 @@
         <f>"PLANNING COURANT  au "&amp;TEXT(K2,"jj/mm/aaaa")</f>
         <v>PLANNING COURANT  au 25/00/Freitag</v>
       </c>
-      <c r="C1" s="300"/>
+      <c r="C1" s="303"/>
       <c r="D1" s="280"/>
       <c r="E1" s="280"/>
       <c r="F1" s="280"/>
       <c r="G1" s="280"/>
       <c r="H1" s="280"/>
       <c r="I1" s="280"/>
-      <c r="J1" s="301"/>
+      <c r="J1" s="304"/>
       <c r="K1" s="249" t="str">
         <f>'1a-Identification Projet'!$L$1</f>
         <v>reference Tableau de bord</v>
@@ -26511,7 +26529,7 @@
       <c r="G2" s="282"/>
       <c r="H2" s="282"/>
       <c r="I2" s="282"/>
-      <c r="J2" s="302"/>
+      <c r="J2" s="305"/>
       <c r="K2" s="238">
         <f>'1a-Identification Projet'!$L$2</f>
         <v>45912</v>
@@ -26530,7 +26548,7 @@
       <c r="G3" s="284"/>
       <c r="H3" s="284"/>
       <c r="I3" s="284"/>
-      <c r="J3" s="303"/>
+      <c r="J3" s="306"/>
       <c r="K3" s="241" t="str">
         <f>'1a-Identification Projet'!$L$3</f>
         <v>Organisation</v>
@@ -26658,25 +26676,25 @@
     </row>
     <row r="7" spans="1:39" ht="24.6">
       <c r="A7"/>
-      <c r="C7" s="304" t="s">
-        <v>266</v>
-      </c>
-      <c r="D7" s="305"/>
-      <c r="E7" s="305"/>
-      <c r="F7" s="305"/>
-      <c r="G7" s="305"/>
-      <c r="H7" s="305"/>
-      <c r="I7" s="306"/>
+      <c r="C7" s="307" t="s">
+        <v>262</v>
+      </c>
+      <c r="D7" s="308"/>
+      <c r="E7" s="308"/>
+      <c r="F7" s="308"/>
+      <c r="G7" s="308"/>
+      <c r="H7" s="308"/>
+      <c r="I7" s="309"/>
       <c r="J7"/>
-      <c r="K7" s="304" t="s">
+      <c r="K7" s="307" t="s">
         <v>95</v>
       </c>
-      <c r="L7" s="305"/>
-      <c r="M7" s="305"/>
-      <c r="N7" s="305"/>
-      <c r="O7" s="305"/>
-      <c r="P7" s="305"/>
-      <c r="Q7" s="306"/>
+      <c r="L7" s="308"/>
+      <c r="M7" s="308"/>
+      <c r="N7" s="308"/>
+      <c r="O7" s="308"/>
+      <c r="P7" s="308"/>
+      <c r="Q7" s="309"/>
       <c r="R7"/>
       <c r="S7"/>
       <c r="T7"/>
@@ -26742,7 +26760,7 @@
         <v>66</v>
       </c>
       <c r="Q8" s="184" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="R8"/>
       <c r="S8"/>
@@ -26800,7 +26818,7 @@
       <c r="P9" s="179"/>
       <c r="Q9" s="185">
         <f>SUM(Q10,Q13,Q22,Q29)</f>
-        <v>16.899999999999999</v>
+        <v>21.7</v>
       </c>
       <c r="R9"/>
       <c r="S9"/>
@@ -26924,7 +26942,7 @@
         <v>204</v>
       </c>
       <c r="Q11" s="180" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="R11"/>
       <c r="S11"/>
@@ -26991,7 +27009,7 @@
         <v>207</v>
       </c>
       <c r="Q12" s="180" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="R12"/>
       <c r="S12"/>
@@ -27302,7 +27320,7 @@
         <v>9</v>
       </c>
       <c r="L17" s="162" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="M17" s="163">
         <v>45940</v>
@@ -27314,7 +27332,7 @@
         <v>7</v>
       </c>
       <c r="P17" s="162" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="Q17" s="180">
         <v>0.6</v>
@@ -27369,7 +27387,7 @@
         <v>10</v>
       </c>
       <c r="L18" s="162" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="M18" s="163">
         <v>45941</v>
@@ -27381,7 +27399,7 @@
         <v>218</v>
       </c>
       <c r="P18" s="162" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="Q18" s="180">
         <v>0.4</v>
@@ -27436,7 +27454,7 @@
         <v>11</v>
       </c>
       <c r="L19" s="162" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="M19" s="163">
         <v>45942</v>
@@ -27503,7 +27521,7 @@
         <v>12</v>
       </c>
       <c r="L20" s="162" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="M20" s="163">
         <v>45944</v>
@@ -27553,10 +27571,10 @@
       <c r="H21" s="162"/>
       <c r="I21" s="161"/>
       <c r="K21" s="161" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="L21" s="162" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="M21" s="163">
         <v>45950</v>
@@ -27566,7 +27584,7 @@
       </c>
       <c r="O21" s="161"/>
       <c r="P21" s="162" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="Q21" s="180">
         <v>0.8</v>
@@ -27731,10 +27749,10 @@
       <c r="H24" s="162"/>
       <c r="I24" s="161"/>
       <c r="K24" s="175" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="L24" s="176" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="M24" s="177">
         <v>45968</v>
@@ -28066,14 +28084,15 @@
         <v>239</v>
       </c>
       <c r="M29" s="166">
-        <v>45992</v>
-      </c>
-      <c r="N29" s="166"/>
+        <v>45998</v>
+      </c>
+      <c r="N29" s="166">
+        <v>46001</v>
+      </c>
       <c r="O29" s="167"/>
       <c r="P29" s="168"/>
       <c r="Q29" s="187">
-        <f>SUM(Q30:Q35)</f>
-        <v>0</v>
+        <v>4.8</v>
       </c>
       <c r="R29"/>
       <c r="S29"/>
@@ -28110,7 +28129,7 @@
         <v>46001</v>
       </c>
       <c r="F30" s="163">
-        <v>45941</v>
+        <v>46002</v>
       </c>
       <c r="G30" s="161" t="s">
         <v>242</v>
@@ -28121,13 +28140,27 @@
       <c r="I30" s="161" t="s">
         <v>205</v>
       </c>
-      <c r="K30" s="161"/>
-      <c r="L30" s="162"/>
-      <c r="M30" s="163"/>
-      <c r="N30" s="163"/>
-      <c r="O30" s="161"/>
-      <c r="P30" s="162"/>
-      <c r="Q30" s="180"/>
+      <c r="K30" s="161">
+        <v>20</v>
+      </c>
+      <c r="L30" s="162" t="s">
+        <v>241</v>
+      </c>
+      <c r="M30" s="163">
+        <v>45998</v>
+      </c>
+      <c r="N30" s="163">
+        <v>45999</v>
+      </c>
+      <c r="O30" s="161" t="s">
+        <v>242</v>
+      </c>
+      <c r="P30" s="162" t="s">
+        <v>212</v>
+      </c>
+      <c r="Q30" s="161" t="s">
+        <v>205</v>
+      </c>
       <c r="R30"/>
       <c r="S30"/>
       <c r="T30"/>
@@ -28153,34 +28186,48 @@
     </row>
     <row r="31" spans="1:39" ht="27" customHeight="1">
       <c r="A31"/>
-      <c r="C31" s="307">
+      <c r="C31" s="300">
         <v>21</v>
       </c>
-      <c r="D31" s="308" t="s">
+      <c r="D31" s="301" t="s">
         <v>243</v>
       </c>
-      <c r="E31" s="309">
+      <c r="E31" s="302">
         <v>46003</v>
       </c>
-      <c r="F31" s="309">
-        <v>45943</v>
+      <c r="F31" s="302">
+        <v>46004</v>
       </c>
       <c r="G31" s="161" t="s">
         <v>244</v>
       </c>
-      <c r="H31" s="308" t="s">
+      <c r="H31" s="301" t="s">
         <v>212</v>
       </c>
-      <c r="I31" s="307" t="s">
+      <c r="I31" s="300" t="s">
         <v>205</v>
       </c>
-      <c r="K31" s="307"/>
-      <c r="L31" s="162"/>
-      <c r="M31" s="163"/>
-      <c r="N31" s="163"/>
-      <c r="O31" s="161"/>
-      <c r="P31" s="162"/>
-      <c r="Q31" s="180"/>
+      <c r="K31" s="300">
+        <v>21</v>
+      </c>
+      <c r="L31" s="301" t="s">
+        <v>243</v>
+      </c>
+      <c r="M31" s="302">
+        <v>45999</v>
+      </c>
+      <c r="N31" s="302">
+        <v>45999</v>
+      </c>
+      <c r="O31" s="161" t="s">
+        <v>244</v>
+      </c>
+      <c r="P31" s="301" t="s">
+        <v>212</v>
+      </c>
+      <c r="Q31" s="300" t="s">
+        <v>226</v>
+      </c>
       <c r="R31"/>
       <c r="S31"/>
       <c r="T31"/>
@@ -28206,22 +28253,24 @@
     </row>
     <row r="32" spans="1:39" ht="27" customHeight="1">
       <c r="A32"/>
-      <c r="C32" s="307"/>
-      <c r="D32" s="308"/>
-      <c r="E32" s="309"/>
-      <c r="F32" s="309"/>
+      <c r="C32" s="300"/>
+      <c r="D32" s="301"/>
+      <c r="E32" s="302"/>
+      <c r="F32" s="302"/>
       <c r="G32" s="161" t="s">
         <v>245</v>
       </c>
-      <c r="H32" s="308"/>
-      <c r="I32" s="307"/>
-      <c r="K32" s="307"/>
-      <c r="L32" s="162"/>
-      <c r="M32" s="163"/>
-      <c r="N32" s="163"/>
-      <c r="O32" s="161"/>
-      <c r="P32" s="162"/>
-      <c r="Q32" s="180"/>
+      <c r="H32" s="301"/>
+      <c r="I32" s="300"/>
+      <c r="K32" s="300"/>
+      <c r="L32" s="301"/>
+      <c r="M32" s="302"/>
+      <c r="N32" s="302"/>
+      <c r="O32" s="161" t="s">
+        <v>245</v>
+      </c>
+      <c r="P32" s="301"/>
+      <c r="Q32" s="300"/>
       <c r="R32"/>
       <c r="S32"/>
       <c r="T32"/>
@@ -28268,13 +28317,27 @@
       <c r="I33" s="161" t="s">
         <v>232</v>
       </c>
-      <c r="K33" s="161"/>
-      <c r="L33" s="162"/>
-      <c r="M33" s="163"/>
-      <c r="N33" s="163"/>
-      <c r="O33" s="161"/>
-      <c r="P33" s="162"/>
-      <c r="Q33" s="180"/>
+      <c r="K33" s="161">
+        <v>22</v>
+      </c>
+      <c r="L33" s="162" t="s">
+        <v>246</v>
+      </c>
+      <c r="M33" s="163">
+        <v>45999</v>
+      </c>
+      <c r="N33" s="163">
+        <v>45999</v>
+      </c>
+      <c r="O33" s="161" t="s">
+        <v>203</v>
+      </c>
+      <c r="P33" s="162" t="s">
+        <v>212</v>
+      </c>
+      <c r="Q33" s="161" t="s">
+        <v>226</v>
+      </c>
       <c r="R33"/>
       <c r="S33"/>
       <c r="T33"/>
@@ -28310,7 +28373,7 @@
         <v>46006</v>
       </c>
       <c r="F34" s="163">
-        <v>45946</v>
+        <v>46007</v>
       </c>
       <c r="G34" s="161" t="s">
         <v>203</v>
@@ -28321,13 +28384,27 @@
       <c r="I34" s="161" t="s">
         <v>205</v>
       </c>
-      <c r="K34" s="161"/>
-      <c r="L34" s="162"/>
-      <c r="M34" s="163"/>
-      <c r="N34" s="163"/>
-      <c r="O34" s="161"/>
-      <c r="P34" s="162"/>
-      <c r="Q34" s="180"/>
+      <c r="K34" s="161">
+        <v>23</v>
+      </c>
+      <c r="L34" s="162" t="s">
+        <v>247</v>
+      </c>
+      <c r="M34" s="163">
+        <v>46000</v>
+      </c>
+      <c r="N34" s="163">
+        <v>46000</v>
+      </c>
+      <c r="O34" s="161" t="s">
+        <v>203</v>
+      </c>
+      <c r="P34" s="162" t="s">
+        <v>212</v>
+      </c>
+      <c r="Q34" s="161" t="s">
+        <v>205</v>
+      </c>
       <c r="R34"/>
       <c r="S34"/>
       <c r="T34"/>
@@ -28363,7 +28440,7 @@
         <v>46009</v>
       </c>
       <c r="F35" s="163">
-        <v>45950</v>
+        <v>46011</v>
       </c>
       <c r="G35" s="161" t="s">
         <v>249</v>
@@ -28374,13 +28451,27 @@
       <c r="I35" s="161" t="s">
         <v>205</v>
       </c>
-      <c r="K35" s="161"/>
-      <c r="L35" s="162"/>
-      <c r="M35" s="163"/>
-      <c r="N35" s="163"/>
-      <c r="O35" s="161"/>
-      <c r="P35" s="162"/>
-      <c r="Q35" s="180"/>
+      <c r="K35" s="161">
+        <v>24</v>
+      </c>
+      <c r="L35" s="162" t="s">
+        <v>248</v>
+      </c>
+      <c r="M35" s="163">
+        <v>46001</v>
+      </c>
+      <c r="N35" s="163">
+        <v>46001</v>
+      </c>
+      <c r="O35" s="161" t="s">
+        <v>249</v>
+      </c>
+      <c r="P35" s="162" t="s">
+        <v>212</v>
+      </c>
+      <c r="Q35" s="161" t="s">
+        <v>205</v>
+      </c>
       <c r="R35"/>
       <c r="S35"/>
       <c r="T35"/>
@@ -35316,7 +35407,18 @@
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
-  <mergeCells count="13">
+  <mergeCells count="18">
+    <mergeCell ref="L31:L32"/>
+    <mergeCell ref="M31:M32"/>
+    <mergeCell ref="N31:N32"/>
+    <mergeCell ref="P31:P32"/>
+    <mergeCell ref="Q31:Q32"/>
+    <mergeCell ref="K1:M1"/>
+    <mergeCell ref="K2:M2"/>
+    <mergeCell ref="K3:M3"/>
+    <mergeCell ref="B1:J3"/>
+    <mergeCell ref="C7:I7"/>
+    <mergeCell ref="K7:Q7"/>
     <mergeCell ref="I31:I32"/>
     <mergeCell ref="K31:K32"/>
     <mergeCell ref="C31:C32"/>
@@ -35324,12 +35426,6 @@
     <mergeCell ref="E31:E32"/>
     <mergeCell ref="F31:F32"/>
     <mergeCell ref="H31:H32"/>
-    <mergeCell ref="K1:M1"/>
-    <mergeCell ref="K2:M2"/>
-    <mergeCell ref="K3:M3"/>
-    <mergeCell ref="B1:J3"/>
-    <mergeCell ref="C7:I7"/>
-    <mergeCell ref="K7:Q7"/>
   </mergeCells>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.23622047244094491" bottom="0.23622047244094491" header="0" footer="0"/>
   <pageSetup paperSize="9" scale="83" firstPageNumber="0" orientation="landscape" r:id="rId1"/>
@@ -35350,7 +35446,7 @@
       <selection activeCell="A11" sqref="A11:H11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.2"/>
   <cols>
     <col min="1" max="1" width="19.6640625" style="3" customWidth="1"/>
     <col min="2" max="2" width="11.44140625" style="3" customWidth="1"/>
@@ -35387,11 +35483,11 @@
       <c r="D2" s="282"/>
       <c r="E2" s="282"/>
       <c r="F2" s="282"/>
-      <c r="G2" s="227">
+      <c r="G2" s="229">
         <f>'1a-Identification Projet'!$L2</f>
         <v>45912</v>
       </c>
-      <c r="H2" s="228"/>
+      <c r="H2" s="230"/>
     </row>
     <row r="3" spans="1:8" ht="16.5" customHeight="1" thickBot="1">
       <c r="A3" s="283"/>
@@ -35400,11 +35496,11 @@
       <c r="D3" s="284"/>
       <c r="E3" s="284"/>
       <c r="F3" s="284"/>
-      <c r="G3" s="229" t="str">
+      <c r="G3" s="231" t="str">
         <f>'1a-Identification Projet'!$L3</f>
         <v>Organisation</v>
       </c>
-      <c r="H3" s="230"/>
+      <c r="H3" s="232"/>
     </row>
     <row r="4" spans="1:8" ht="12.75" customHeight="1">
       <c r="B4" s="26"/>
@@ -35429,7 +35525,7 @@
     </row>
     <row r="8" spans="1:8" ht="113.4" customHeight="1">
       <c r="A8" s="316" t="s">
-        <v>339</v>
+        <v>333</v>
       </c>
       <c r="B8" s="316"/>
       <c r="C8" s="316"/>
@@ -35456,7 +35552,7 @@
     </row>
     <row r="11" spans="1:8" ht="154.19999999999999" customHeight="1">
       <c r="A11" s="317" t="s">
-        <v>340</v>
+        <v>334</v>
       </c>
       <c r="B11" s="317"/>
       <c r="C11" s="317"/>
@@ -35483,7 +35579,7 @@
     </row>
     <row r="14" spans="1:8" ht="93.75" customHeight="1">
       <c r="A14" s="310" t="s">
-        <v>341</v>
+        <v>335</v>
       </c>
       <c r="B14" s="311"/>
       <c r="C14" s="311"/>
@@ -35521,7 +35617,7 @@
       <selection activeCell="J32" sqref="J32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.2"/>
   <cols>
     <col min="1" max="1" width="18" customWidth="1"/>
     <col min="2" max="2" width="16.88671875" customWidth="1"/>
@@ -35560,7 +35656,7 @@
       <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="13.2" outlineLevelRow="2"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.2" outlineLevelRow="2"/>
   <cols>
     <col min="1" max="1" width="26.33203125" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11.44140625" style="3" customWidth="1"/>
@@ -35581,11 +35677,11 @@
       <c r="D1" s="109"/>
       <c r="E1" s="109"/>
       <c r="F1" s="109"/>
-      <c r="G1" s="225" t="str">
+      <c r="G1" s="227" t="str">
         <f>'1a-Identification Projet'!$L1</f>
         <v>reference Tableau de bord</v>
       </c>
-      <c r="H1" s="226"/>
+      <c r="H1" s="228"/>
     </row>
     <row r="2" spans="1:15" ht="12.75" customHeight="1">
       <c r="A2" s="106"/>
@@ -35594,11 +35690,11 @@
       <c r="D2" s="110"/>
       <c r="E2" s="110"/>
       <c r="F2" s="110"/>
-      <c r="G2" s="227">
+      <c r="G2" s="229">
         <f>'1a-Identification Projet'!$L2</f>
         <v>45912</v>
       </c>
-      <c r="H2" s="228"/>
+      <c r="H2" s="230"/>
     </row>
     <row r="3" spans="1:15" ht="16.5" customHeight="1" thickBot="1">
       <c r="A3" s="1"/>
@@ -35607,11 +35703,11 @@
       <c r="D3" s="111"/>
       <c r="E3" s="111"/>
       <c r="F3" s="111"/>
-      <c r="G3" s="229" t="str">
+      <c r="G3" s="231" t="str">
         <f>'1a-Identification Projet'!$L3</f>
         <v>Organisation</v>
       </c>
-      <c r="H3" s="230"/>
+      <c r="H3" s="232"/>
     </row>
     <row r="4" spans="1:15" ht="12.75" customHeight="1">
       <c r="B4" s="26"/>
@@ -35641,16 +35737,16 @@
       <c r="H7" s="127"/>
     </row>
     <row r="8" spans="1:15" ht="96" customHeight="1">
-      <c r="A8" s="231" t="s">
+      <c r="A8" s="233" t="s">
         <v>101</v>
       </c>
-      <c r="B8" s="231"/>
-      <c r="C8" s="231"/>
-      <c r="D8" s="231"/>
-      <c r="E8" s="231"/>
-      <c r="F8" s="231"/>
-      <c r="G8" s="231"/>
-      <c r="H8" s="231"/>
+      <c r="B8" s="233"/>
+      <c r="C8" s="233"/>
+      <c r="D8" s="233"/>
+      <c r="E8" s="233"/>
+      <c r="F8" s="233"/>
+      <c r="G8" s="233"/>
+      <c r="H8" s="233"/>
     </row>
     <row r="9" spans="1:15" ht="13.8" thickBot="1">
       <c r="A9" s="76" t="s">
@@ -35707,10 +35803,10 @@
       <c r="F11" s="124" t="s">
         <v>104</v>
       </c>
-      <c r="G11" s="232" t="s">
+      <c r="G11" s="225" t="s">
         <v>105</v>
       </c>
-      <c r="H11" s="233"/>
+      <c r="H11" s="234"/>
     </row>
     <row r="12" spans="1:15" ht="41.4" outlineLevel="2">
       <c r="A12" s="122" t="s">
@@ -35731,10 +35827,10 @@
       <c r="F12" s="123" t="s">
         <v>109</v>
       </c>
-      <c r="G12" s="232" t="s">
+      <c r="G12" s="225" t="s">
         <v>110</v>
       </c>
-      <c r="H12" s="234"/>
+      <c r="H12" s="226"/>
       <c r="I12" s="4"/>
       <c r="J12" s="4"/>
       <c r="K12" s="4"/>
@@ -35760,10 +35856,10 @@
         <v>113</v>
       </c>
       <c r="F13" s="124"/>
-      <c r="G13" s="232" t="s">
+      <c r="G13" s="225" t="s">
         <v>114</v>
       </c>
-      <c r="H13" s="234"/>
+      <c r="H13" s="226"/>
     </row>
     <row r="14" spans="1:15" s="4" customFormat="1" ht="27.6" outlineLevel="2">
       <c r="A14" s="122" t="s">
@@ -35784,10 +35880,10 @@
       <c r="F14" s="124" t="s">
         <v>118</v>
       </c>
-      <c r="G14" s="232" t="s">
+      <c r="G14" s="225" t="s">
         <v>119</v>
       </c>
-      <c r="H14" s="234"/>
+      <c r="H14" s="226"/>
     </row>
     <row r="15" spans="1:15" s="4" customFormat="1" ht="41.4" outlineLevel="2">
       <c r="A15" s="122" t="s">
@@ -35808,10 +35904,10 @@
       <c r="F15" s="123" t="s">
         <v>123</v>
       </c>
-      <c r="G15" s="232" t="s">
+      <c r="G15" s="225" t="s">
         <v>124</v>
       </c>
-      <c r="H15" s="234"/>
+      <c r="H15" s="226"/>
       <c r="I15" s="3"/>
       <c r="J15" s="3"/>
       <c r="K15" s="3"/>
@@ -35839,10 +35935,10 @@
       <c r="F16" s="124" t="s">
         <v>128</v>
       </c>
-      <c r="G16" s="232" t="s">
+      <c r="G16" s="225" t="s">
         <v>129</v>
       </c>
-      <c r="H16" s="234"/>
+      <c r="H16" s="226"/>
     </row>
     <row r="17" spans="1:8" ht="41.4" outlineLevel="2">
       <c r="A17" s="122" t="s">
@@ -35863,10 +35959,10 @@
       <c r="F17" s="123" t="s">
         <v>133</v>
       </c>
-      <c r="G17" s="232" t="s">
+      <c r="G17" s="225" t="s">
         <v>134</v>
       </c>
-      <c r="H17" s="234"/>
+      <c r="H17" s="226"/>
     </row>
     <row r="18" spans="1:8" ht="41.4">
       <c r="A18" s="122" t="s">
@@ -35887,10 +35983,10 @@
       <c r="F18" s="123" t="s">
         <v>138</v>
       </c>
-      <c r="G18" s="232" t="s">
+      <c r="G18" s="225" t="s">
         <v>139</v>
       </c>
-      <c r="H18" s="234"/>
+      <c r="H18" s="226"/>
     </row>
     <row r="19" spans="1:8" ht="27.6">
       <c r="A19" s="122" t="s">
@@ -35911,10 +36007,10 @@
       <c r="F19" s="123" t="s">
         <v>143</v>
       </c>
-      <c r="G19" s="232" t="s">
+      <c r="G19" s="225" t="s">
         <v>144</v>
       </c>
-      <c r="H19" s="234"/>
+      <c r="H19" s="226"/>
     </row>
     <row r="20" spans="1:8" ht="27.6">
       <c r="A20" s="122" t="s">
@@ -35935,10 +36031,10 @@
       <c r="F20" s="123" t="s">
         <v>148</v>
       </c>
-      <c r="G20" s="232" t="s">
+      <c r="G20" s="225" t="s">
         <v>149</v>
       </c>
-      <c r="H20" s="234"/>
+      <c r="H20" s="226"/>
     </row>
     <row r="21" spans="1:8" ht="27.6">
       <c r="A21" s="122" t="s">
@@ -35959,10 +36055,10 @@
       <c r="F21" s="123" t="s">
         <v>153</v>
       </c>
-      <c r="G21" s="232" t="s">
+      <c r="G21" s="225" t="s">
         <v>154</v>
       </c>
-      <c r="H21" s="234"/>
+      <c r="H21" s="226"/>
     </row>
     <row r="22" spans="1:8" ht="27.6">
       <c r="A22" s="122" t="s">
@@ -35983,10 +36079,10 @@
       <c r="F22" s="123" t="s">
         <v>158</v>
       </c>
-      <c r="G22" s="232" t="s">
+      <c r="G22" s="225" t="s">
         <v>159</v>
       </c>
-      <c r="H22" s="234"/>
+      <c r="H22" s="226"/>
     </row>
     <row r="23" spans="1:8" ht="27.6">
       <c r="A23" s="122" t="s">
@@ -36007,10 +36103,10 @@
       <c r="F23" s="124" t="s">
         <v>162</v>
       </c>
-      <c r="G23" s="232" t="s">
+      <c r="G23" s="225" t="s">
         <v>163</v>
       </c>
-      <c r="H23" s="234"/>
+      <c r="H23" s="226"/>
     </row>
     <row r="24" spans="1:8" ht="13.8">
       <c r="A24" s="122" t="s">
@@ -36031,10 +36127,10 @@
       <c r="F24" s="124" t="s">
         <v>167</v>
       </c>
-      <c r="G24" s="232" t="s">
+      <c r="G24" s="225" t="s">
         <v>168</v>
       </c>
-      <c r="H24" s="234"/>
+      <c r="H24" s="226"/>
     </row>
     <row r="25" spans="1:8" ht="27.6">
       <c r="A25" s="122" t="s">
@@ -36055,10 +36151,10 @@
       <c r="F25" s="124" t="s">
         <v>172</v>
       </c>
-      <c r="G25" s="232" t="s">
+      <c r="G25" s="225" t="s">
         <v>173</v>
       </c>
-      <c r="H25" s="234"/>
+      <c r="H25" s="226"/>
     </row>
     <row r="26" spans="1:8" ht="13.8">
       <c r="A26" s="122" t="s">
@@ -36079,10 +36175,10 @@
       <c r="F26" s="124" t="s">
         <v>177</v>
       </c>
-      <c r="G26" s="232" t="s">
+      <c r="G26" s="225" t="s">
         <v>178</v>
       </c>
-      <c r="H26" s="234"/>
+      <c r="H26" s="226"/>
     </row>
     <row r="27" spans="1:8" ht="27.6">
       <c r="A27" s="122" t="s">
@@ -36103,10 +36199,10 @@
       <c r="F27" s="123" t="s">
         <v>182</v>
       </c>
-      <c r="G27" s="232" t="s">
+      <c r="G27" s="225" t="s">
         <v>183</v>
       </c>
-      <c r="H27" s="234"/>
+      <c r="H27" s="226"/>
     </row>
     <row r="28" spans="1:8" ht="13.8">
       <c r="A28" s="122" t="s">
@@ -36127,10 +36223,10 @@
       <c r="F28" s="124" t="s">
         <v>187</v>
       </c>
-      <c r="G28" s="232" t="s">
+      <c r="G28" s="225" t="s">
         <v>188</v>
       </c>
-      <c r="H28" s="234"/>
+      <c r="H28" s="226"/>
     </row>
     <row r="29" spans="1:8" ht="13.8">
       <c r="A29" s="122" t="s">
@@ -36151,10 +36247,10 @@
       <c r="F29" s="124" t="s">
         <v>192</v>
       </c>
-      <c r="G29" s="232" t="s">
+      <c r="G29" s="225" t="s">
         <v>193</v>
       </c>
-      <c r="H29" s="234"/>
+      <c r="H29" s="226"/>
     </row>
     <row r="30" spans="1:8" ht="13.8">
       <c r="A30" s="122" t="s">
@@ -36169,11 +36265,26 @@
       </c>
       <c r="E30" s="124"/>
       <c r="F30" s="124"/>
-      <c r="G30" s="232"/>
-      <c r="H30" s="234"/>
+      <c r="G30" s="225"/>
+      <c r="H30" s="226"/>
     </row>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="G1:H1"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="G3:H3"/>
+    <mergeCell ref="A8:H8"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="G19:H19"/>
+    <mergeCell ref="G20:H20"/>
+    <mergeCell ref="G21:H21"/>
     <mergeCell ref="G27:H27"/>
     <mergeCell ref="G28:H28"/>
     <mergeCell ref="G29:H29"/>
@@ -36183,21 +36294,6 @@
     <mergeCell ref="G24:H24"/>
     <mergeCell ref="G25:H25"/>
     <mergeCell ref="G26:H26"/>
-    <mergeCell ref="G17:H17"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="G19:H19"/>
-    <mergeCell ref="G20:H20"/>
-    <mergeCell ref="G21:H21"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="G16:H16"/>
-    <mergeCell ref="G1:H1"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="G3:H3"/>
-    <mergeCell ref="A8:H8"/>
-    <mergeCell ref="G11:H11"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.23622047244094491" bottom="0.23622047244094491" header="0" footer="0"/>
@@ -36215,7 +36311,7 @@
       <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.5546875" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="11.5546875" defaultRowHeight="13.2"/>
   <cols>
     <col min="1" max="16384" width="11.5546875" style="172"/>
   </cols>
@@ -36235,7 +36331,7 @@
       <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.2"/>
   <cols>
     <col min="1" max="1" width="1.6640625" style="3" customWidth="1"/>
     <col min="2" max="16384" width="11.44140625" style="3"/>
@@ -36433,7 +36529,7 @@
       <selection activeCell="J65" sqref="J65"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.2"/>
   <cols>
     <col min="1" max="1" width="1.6640625" style="3" customWidth="1"/>
     <col min="2" max="16384" width="11.44140625" style="3"/>
@@ -37323,7 +37419,7 @@
       <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.2"/>
   <cols>
     <col min="1" max="1" width="1.6640625" style="3" customWidth="1"/>
     <col min="2" max="16384" width="11.44140625" style="3"/>
@@ -37943,11 +38039,11 @@
   </sheetPr>
   <dimension ref="A1:O35"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A67" zoomScale="79" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
+    <sheetView showGridLines="0" topLeftCell="A23" zoomScale="115" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.2"/>
   <cols>
     <col min="1" max="1" width="1.6640625" style="3" customWidth="1"/>
     <col min="2" max="2" width="14.33203125" style="3" customWidth="1"/>
@@ -38654,7 +38750,7 @@
         <v>46001</v>
       </c>
       <c r="E27" s="142">
-        <v>45941</v>
+        <v>46002</v>
       </c>
       <c r="F27" s="143" t="s">
         <v>242</v>
@@ -38684,7 +38780,7 @@
         <v>46003</v>
       </c>
       <c r="E28" s="255">
-        <v>45943</v>
+        <v>46004</v>
       </c>
       <c r="F28" s="150" t="s">
         <v>244</v>
@@ -38732,7 +38828,7 @@
         <v>46003</v>
       </c>
       <c r="E30" s="142">
-        <v>45943</v>
+        <v>46004</v>
       </c>
       <c r="F30" s="143" t="s">
         <v>203</v>
@@ -38762,7 +38858,7 @@
         <v>46006</v>
       </c>
       <c r="E31" s="142">
-        <v>45946</v>
+        <v>46007</v>
       </c>
       <c r="F31" s="143" t="s">
         <v>203</v>
@@ -38792,7 +38888,7 @@
         <v>46009</v>
       </c>
       <c r="E32" s="142">
-        <v>45950</v>
+        <v>46011</v>
       </c>
       <c r="F32" s="143" t="s">
         <v>249</v>
@@ -38885,13 +38981,13 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:K82"/>
+  <dimension ref="A1:K75"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A47" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="60" workbookViewId="0">
-      <selection activeCell="B57" sqref="B57"/>
+    <sheetView showGridLines="0" topLeftCell="A53" zoomScale="84" zoomScaleNormal="80" zoomScalePageLayoutView="60" workbookViewId="0">
+      <selection activeCell="A75" sqref="A75"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="13.2" outlineLevelRow="1"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.2" outlineLevelRow="1"/>
   <cols>
     <col min="1" max="1" width="88.6640625" style="20" customWidth="1"/>
     <col min="2" max="2" width="85.33203125" style="20" customWidth="1"/>
@@ -38979,10 +39075,10 @@
     </row>
     <row r="8" spans="1:11" ht="31.2" outlineLevel="1">
       <c r="A8" s="107" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="B8" s="107" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="15.6" outlineLevel="1">
@@ -39017,7 +39113,7 @@
     </row>
     <row r="15" spans="1:11" ht="31.2" outlineLevel="1">
       <c r="A15" s="107" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="B15" s="107"/>
     </row>
@@ -39053,10 +39149,10 @@
     </row>
     <row r="22" spans="1:2" ht="46.8">
       <c r="A22" s="107" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="B22" s="107" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
     </row>
     <row r="23" spans="1:2" ht="15.6">
@@ -39091,16 +39187,16 @@
     </row>
     <row r="29" spans="1:2" ht="31.2">
       <c r="A29" s="107" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="B29" s="107" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
     </row>
     <row r="30" spans="1:2" ht="15.6">
       <c r="A30" s="107"/>
       <c r="B30" s="107" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
     </row>
     <row r="31" spans="1:2" ht="15.6">
@@ -39131,10 +39227,10 @@
     </row>
     <row r="36" spans="1:2" ht="31.2">
       <c r="A36" s="107" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="B36" s="107" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
     </row>
     <row r="37" spans="1:2" ht="15.6">
@@ -39155,7 +39251,7 @@
     </row>
     <row r="41" spans="1:2" ht="18" thickBot="1">
       <c r="A41" s="47" t="s">
-        <v>257</v>
+        <v>340</v>
       </c>
       <c r="B41" s="48"/>
     </row>
@@ -39170,7 +39266,7 @@
     <row r="43" spans="1:2" ht="31.2">
       <c r="A43" s="107"/>
       <c r="B43" s="107" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
     </row>
     <row r="44" spans="1:2" ht="15.6">
@@ -39191,7 +39287,7 @@
     </row>
     <row r="48" spans="1:2" ht="18" thickBot="1">
       <c r="A48" s="47" t="s">
-        <v>258</v>
+        <v>341</v>
       </c>
       <c r="B48" s="48"/>
     </row>
@@ -39205,13 +39301,13 @@
     </row>
     <row r="50" spans="1:2" ht="31.2">
       <c r="A50" s="107" t="s">
-        <v>297</v>
+        <v>293</v>
       </c>
       <c r="B50" s="107"/>
     </row>
     <row r="51" spans="1:2" ht="15.6">
       <c r="A51" s="107" t="s">
-        <v>298</v>
+        <v>294</v>
       </c>
       <c r="B51" s="107"/>
     </row>
@@ -39229,7 +39325,7 @@
     </row>
     <row r="55" spans="1:2" ht="18" thickBot="1">
       <c r="A55" s="47" t="s">
-        <v>259</v>
+        <v>339</v>
       </c>
       <c r="B55" s="48"/>
     </row>
@@ -39244,7 +39340,7 @@
     <row r="57" spans="1:2" ht="31.2">
       <c r="A57" s="107"/>
       <c r="B57" s="107" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
     </row>
     <row r="58" spans="1:2" ht="15.6">
@@ -39265,7 +39361,7 @@
     </row>
     <row r="62" spans="1:2" ht="18" thickBot="1">
       <c r="A62" s="47" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="B62" s="48"/>
     </row>
@@ -39277,13 +39373,19 @@
         <v>5</v>
       </c>
     </row>
-    <row r="64" spans="1:2" ht="15.6">
-      <c r="A64" s="107"/>
-      <c r="B64" s="107"/>
-    </row>
-    <row r="65" spans="1:2" ht="15.6">
+    <row r="64" spans="1:2" ht="31.2">
+      <c r="A64" s="107" t="s">
+        <v>344</v>
+      </c>
+      <c r="B64" s="107" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" ht="31.2">
       <c r="A65" s="107"/>
-      <c r="B65" s="107"/>
+      <c r="B65" s="107" t="s">
+        <v>343</v>
+      </c>
     </row>
     <row r="66" spans="1:2" ht="15.6">
       <c r="A66" s="107"/>
@@ -39299,7 +39401,7 @@
     </row>
     <row r="69" spans="1:2" ht="18" thickBot="1">
       <c r="A69" s="47" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="B69" s="48"/>
     </row>
@@ -39312,15 +39414,21 @@
       </c>
     </row>
     <row r="71" spans="1:2" ht="15.6">
-      <c r="A71" s="107"/>
+      <c r="A71" s="107" t="s">
+        <v>345</v>
+      </c>
       <c r="B71" s="107"/>
     </row>
     <row r="72" spans="1:2" ht="15.6">
-      <c r="A72" s="107"/>
+      <c r="A72" s="107" t="s">
+        <v>346</v>
+      </c>
       <c r="B72" s="107"/>
     </row>
     <row r="73" spans="1:2" ht="15.6">
-      <c r="A73" s="107"/>
+      <c r="A73" s="107" t="s">
+        <v>347</v>
+      </c>
       <c r="B73" s="107"/>
     </row>
     <row r="74" spans="1:2" ht="15">
@@ -39330,40 +39438,6 @@
     <row r="75" spans="1:2" ht="15">
       <c r="A75" s="33"/>
       <c r="B75" s="35"/>
-    </row>
-    <row r="76" spans="1:2" ht="18" thickBot="1">
-      <c r="A76" s="47" t="s">
-        <v>262</v>
-      </c>
-      <c r="B76" s="48"/>
-    </row>
-    <row r="77" spans="1:2" ht="16.2" thickBot="1">
-      <c r="A77" s="169" t="s">
-        <v>4</v>
-      </c>
-      <c r="B77" s="171" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="78" spans="1:2" ht="15.6">
-      <c r="A78" s="107"/>
-      <c r="B78" s="107"/>
-    </row>
-    <row r="79" spans="1:2" ht="15.6">
-      <c r="A79" s="107"/>
-      <c r="B79" s="107"/>
-    </row>
-    <row r="80" spans="1:2" ht="15.6">
-      <c r="A80" s="107"/>
-      <c r="B80" s="107"/>
-    </row>
-    <row r="81" spans="1:2" ht="15">
-      <c r="A81" s="32"/>
-      <c r="B81" s="34"/>
-    </row>
-    <row r="82" spans="1:2" ht="15">
-      <c r="A82" s="33"/>
-      <c r="B82" s="35"/>
     </row>
   </sheetData>
   <sheetProtection selectLockedCells="1" selectUnlockedCells="1"/>
@@ -39379,13 +39453,13 @@
   <sheetPr codeName="Feuil15">
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:BH19"/>
+  <dimension ref="A1:BH20"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScale="82" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView showGridLines="0" zoomScale="124" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="13.2"/>
+  <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.2"/>
   <cols>
     <col min="1" max="1" width="7.88671875" style="3" customWidth="1"/>
     <col min="2" max="2" width="58.44140625" style="3" customWidth="1"/>
@@ -39401,9 +39475,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:60" ht="13.5" customHeight="1">
-      <c r="A1" s="257" t="str">
+      <c r="A1" s="257" t="e">
         <f>"LISTE DES ACTIONS au "&amp;TEXT(I2,"jj/mm/aaaa")</f>
-        <v>LISTE DES ACTIONS au 25/00/Freitag</v>
+        <v>#VALUE!</v>
       </c>
       <c r="B1" s="258"/>
       <c r="C1" s="258"/>
@@ -39412,11 +39486,11 @@
       <c r="F1" s="258"/>
       <c r="G1" s="258"/>
       <c r="H1" s="259"/>
-      <c r="I1" s="225" t="str">
+      <c r="I1" s="227" t="str">
         <f>'1a-Identification Projet'!$L1</f>
         <v>reference Tableau de bord</v>
       </c>
-      <c r="J1" s="226"/>
+      <c r="J1" s="228"/>
     </row>
     <row r="2" spans="1:60" ht="12.75" customHeight="1">
       <c r="A2" s="260"/>
@@ -39427,11 +39501,11 @@
       <c r="F2" s="261"/>
       <c r="G2" s="261"/>
       <c r="H2" s="262"/>
-      <c r="I2" s="227">
+      <c r="I2" s="229">
         <f>'1a-Identification Projet'!$L2</f>
         <v>45912</v>
       </c>
-      <c r="J2" s="228"/>
+      <c r="J2" s="230"/>
     </row>
     <row r="3" spans="1:60" ht="16.5" customHeight="1" thickBot="1">
       <c r="A3" s="263"/>
@@ -39442,11 +39516,11 @@
       <c r="F3" s="264"/>
       <c r="G3" s="264"/>
       <c r="H3" s="265"/>
-      <c r="I3" s="229" t="str">
+      <c r="I3" s="231" t="str">
         <f>'1a-Identification Projet'!$L3</f>
         <v>Organisation</v>
       </c>
-      <c r="J3" s="230"/>
+      <c r="J3" s="232"/>
     </row>
     <row r="4" spans="1:60" ht="12.75" customHeight="1" thickBot="1">
       <c r="B4" s="26"/>
@@ -39540,10 +39614,10 @@
         <v>1</v>
       </c>
       <c r="B6" s="78" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="C6" s="80" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="D6" s="81">
         <v>45908</v>
@@ -39551,7 +39625,7 @@
       <c r="E6" s="81"/>
       <c r="F6" s="81"/>
       <c r="G6" s="81" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="H6" s="81">
         <v>45908</v>
@@ -39560,7 +39634,7 @@
         <v>45908</v>
       </c>
       <c r="J6" s="82" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="K6" s="27"/>
       <c r="L6" s="27"/>
@@ -39618,10 +39692,10 @@
         <v>2</v>
       </c>
       <c r="B7" s="78" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="C7" s="80" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="D7" s="81">
         <v>45910</v>
@@ -39629,7 +39703,7 @@
       <c r="E7" s="81"/>
       <c r="F7" s="81"/>
       <c r="G7" s="80" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="H7" s="81">
         <v>45910</v>
@@ -39694,7 +39768,7 @@
         <v>3</v>
       </c>
       <c r="B8" s="84" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="C8" s="79" t="s">
         <v>59</v>
@@ -39705,7 +39779,7 @@
       <c r="E8" s="85"/>
       <c r="F8" s="85"/>
       <c r="G8" s="79" t="s">
-        <v>320</v>
+        <v>314</v>
       </c>
       <c r="H8" s="86">
         <v>46003</v>
@@ -39768,10 +39842,10 @@
         <v>4</v>
       </c>
       <c r="B9" s="78" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="C9" s="80" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="D9" s="81">
         <v>45949</v>
@@ -39783,7 +39857,7 @@
         <v>45950</v>
       </c>
       <c r="G9" s="81" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="H9" s="81">
         <v>45950</v>
@@ -39848,10 +39922,10 @@
         <v>5</v>
       </c>
       <c r="B10" s="84" t="s">
-        <v>321</v>
+        <v>348</v>
       </c>
       <c r="C10" s="79" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="D10" s="85">
         <v>45968</v>
@@ -39859,7 +39933,7 @@
       <c r="E10" s="85"/>
       <c r="F10" s="85"/>
       <c r="G10" s="79" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="H10" s="85">
         <v>45970</v>
@@ -39920,16 +39994,28 @@
       <c r="BH10" s="3"/>
     </row>
     <row r="11" spans="1:60" s="23" customFormat="1" ht="15">
-      <c r="A11" s="196"/>
-      <c r="B11" s="204"/>
-      <c r="C11" s="198"/>
-      <c r="D11" s="199"/>
-      <c r="E11" s="199"/>
-      <c r="F11" s="199"/>
-      <c r="G11" s="198"/>
-      <c r="H11" s="205"/>
-      <c r="I11" s="202"/>
-      <c r="J11" s="197"/>
+      <c r="A11" s="83">
+        <v>6</v>
+      </c>
+      <c r="B11" s="84" t="s">
+        <v>349</v>
+      </c>
+      <c r="C11" s="79" t="s">
+        <v>350</v>
+      </c>
+      <c r="D11" s="85">
+        <v>45992</v>
+      </c>
+      <c r="E11" s="85"/>
+      <c r="F11" s="85"/>
+      <c r="G11" s="79" t="s">
+        <v>314</v>
+      </c>
+      <c r="H11" s="85">
+        <v>45998</v>
+      </c>
+      <c r="I11" s="85"/>
+      <c r="J11" s="84"/>
       <c r="K11" s="27"/>
       <c r="L11" s="27"/>
       <c r="M11" s="27"/>
@@ -39989,7 +40075,7 @@
       <c r="E12" s="199"/>
       <c r="F12" s="199"/>
       <c r="G12" s="198"/>
-      <c r="H12" s="201"/>
+      <c r="H12" s="205"/>
       <c r="I12" s="202"/>
       <c r="J12" s="197"/>
       <c r="K12" s="27"/>
@@ -40043,29 +40129,29 @@
       <c r="BG12" s="3"/>
       <c r="BH12" s="3"/>
     </row>
-    <row r="13" spans="1:60" s="23" customFormat="1">
-      <c r="A13" s="3"/>
-      <c r="B13" s="3"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="3"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="3"/>
-      <c r="H13" s="3"/>
-      <c r="I13" s="3"/>
-      <c r="J13" s="3"/>
-      <c r="K13" s="3"/>
-      <c r="L13" s="3"/>
-      <c r="M13" s="3"/>
-      <c r="N13" s="3"/>
-      <c r="O13" s="3"/>
-      <c r="P13" s="3"/>
-      <c r="Q13" s="3"/>
-      <c r="R13" s="3"/>
-      <c r="S13" s="3"/>
-      <c r="T13" s="3"/>
-      <c r="U13" s="3"/>
-      <c r="V13" s="3"/>
+    <row r="13" spans="1:60" s="23" customFormat="1" ht="15">
+      <c r="A13" s="196"/>
+      <c r="B13" s="204"/>
+      <c r="C13" s="198"/>
+      <c r="D13" s="199"/>
+      <c r="E13" s="199"/>
+      <c r="F13" s="199"/>
+      <c r="G13" s="198"/>
+      <c r="H13" s="201"/>
+      <c r="I13" s="202"/>
+      <c r="J13" s="197"/>
+      <c r="K13" s="27"/>
+      <c r="L13" s="27"/>
+      <c r="M13" s="27"/>
+      <c r="N13" s="27"/>
+      <c r="O13" s="27"/>
+      <c r="P13" s="27"/>
+      <c r="Q13" s="27"/>
+      <c r="R13" s="27"/>
+      <c r="S13" s="27"/>
+      <c r="T13" s="28"/>
+      <c r="U13" s="28"/>
+      <c r="V13" s="28"/>
       <c r="W13" s="3"/>
       <c r="X13" s="3"/>
       <c r="Y13" s="3"/>
@@ -40105,20 +40191,70 @@
       <c r="BG13" s="3"/>
       <c r="BH13" s="3"/>
     </row>
-    <row r="14" spans="1:60">
-      <c r="F14" s="22"/>
-    </row>
-    <row r="16" spans="1:60">
-      <c r="A16" s="194"/>
-      <c r="B16" s="194"/>
-      <c r="C16" s="194"/>
-      <c r="D16" s="194"/>
-      <c r="E16" s="195"/>
-      <c r="F16" s="195"/>
-      <c r="G16" s="194"/>
-      <c r="H16" s="194"/>
-      <c r="I16" s="194"/>
-      <c r="J16" s="194"/>
+    <row r="14" spans="1:60" s="23" customFormat="1">
+      <c r="A14" s="3"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="4"/>
+      <c r="F14" s="4"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
+      <c r="I14" s="3"/>
+      <c r="J14" s="3"/>
+      <c r="K14" s="3"/>
+      <c r="L14" s="3"/>
+      <c r="M14" s="3"/>
+      <c r="N14" s="3"/>
+      <c r="O14" s="3"/>
+      <c r="P14" s="3"/>
+      <c r="Q14" s="3"/>
+      <c r="R14" s="3"/>
+      <c r="S14" s="3"/>
+      <c r="T14" s="3"/>
+      <c r="U14" s="3"/>
+      <c r="V14" s="3"/>
+      <c r="W14" s="3"/>
+      <c r="X14" s="3"/>
+      <c r="Y14" s="3"/>
+      <c r="Z14" s="3"/>
+      <c r="AA14" s="3"/>
+      <c r="AB14" s="3"/>
+      <c r="AC14" s="3"/>
+      <c r="AD14" s="3"/>
+      <c r="AE14" s="3"/>
+      <c r="AF14" s="3"/>
+      <c r="AG14" s="3"/>
+      <c r="AH14" s="3"/>
+      <c r="AI14" s="3"/>
+      <c r="AJ14" s="3"/>
+      <c r="AK14" s="3"/>
+      <c r="AL14" s="3"/>
+      <c r="AM14" s="3"/>
+      <c r="AN14" s="3"/>
+      <c r="AO14" s="3"/>
+      <c r="AP14" s="3"/>
+      <c r="AQ14" s="3"/>
+      <c r="AR14" s="3"/>
+      <c r="AS14" s="3"/>
+      <c r="AT14" s="3"/>
+      <c r="AU14" s="3"/>
+      <c r="AV14" s="3"/>
+      <c r="AW14" s="3"/>
+      <c r="AX14" s="3"/>
+      <c r="AY14" s="3"/>
+      <c r="AZ14" s="3"/>
+      <c r="BA14" s="3"/>
+      <c r="BB14" s="3"/>
+      <c r="BC14" s="3"/>
+      <c r="BD14" s="3"/>
+      <c r="BE14" s="3"/>
+      <c r="BF14" s="3"/>
+      <c r="BG14" s="3"/>
+      <c r="BH14" s="3"/>
+    </row>
+    <row r="15" spans="1:60">
+      <c r="F15" s="22"/>
     </row>
     <row r="17" spans="1:10">
       <c r="A17" s="194"/>
@@ -40133,16 +40269,16 @@
       <c r="J17" s="194"/>
     </row>
     <row r="18" spans="1:10">
-      <c r="A18" s="196"/>
-      <c r="B18" s="197"/>
-      <c r="C18" s="198"/>
-      <c r="D18" s="199"/>
-      <c r="E18" s="199"/>
-      <c r="F18" s="199"/>
-      <c r="G18" s="199"/>
-      <c r="H18" s="199"/>
-      <c r="I18" s="199"/>
-      <c r="J18" s="200"/>
+      <c r="A18" s="194"/>
+      <c r="B18" s="194"/>
+      <c r="C18" s="194"/>
+      <c r="D18" s="194"/>
+      <c r="E18" s="195"/>
+      <c r="F18" s="195"/>
+      <c r="G18" s="194"/>
+      <c r="H18" s="194"/>
+      <c r="I18" s="194"/>
+      <c r="J18" s="194"/>
     </row>
     <row r="19" spans="1:10">
       <c r="A19" s="196"/>
@@ -40151,10 +40287,22 @@
       <c r="D19" s="199"/>
       <c r="E19" s="199"/>
       <c r="F19" s="199"/>
-      <c r="G19" s="198"/>
-      <c r="H19" s="201"/>
-      <c r="I19" s="202"/>
-      <c r="J19" s="197"/>
+      <c r="G19" s="199"/>
+      <c r="H19" s="199"/>
+      <c r="I19" s="199"/>
+      <c r="J19" s="200"/>
+    </row>
+    <row r="20" spans="1:10">
+      <c r="A20" s="196"/>
+      <c r="B20" s="197"/>
+      <c r="C20" s="198"/>
+      <c r="D20" s="199"/>
+      <c r="E20" s="199"/>
+      <c r="F20" s="199"/>
+      <c r="G20" s="198"/>
+      <c r="H20" s="201"/>
+      <c r="I20" s="202"/>
+      <c r="J20" s="197"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -40163,7 +40311,7 @@
     <mergeCell ref="I3:J3"/>
     <mergeCell ref="A1:H3"/>
   </mergeCells>
-  <conditionalFormatting sqref="A6:J10">
+  <conditionalFormatting sqref="A6:J11">
     <cfRule type="expression" dxfId="8" priority="1" stopIfTrue="1">
       <formula>IF($G6="Done",TRUE,FALSE)</formula>
     </cfRule>
@@ -40174,30 +40322,30 @@
       <formula>IF($G6="Pending",TRUE,FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A12:J12">
+  <conditionalFormatting sqref="A13:J13">
     <cfRule type="expression" dxfId="5" priority="31" stopIfTrue="1">
-      <formula>IF($G12="Done",TRUE,FALSE)</formula>
+      <formula>IF($G13="Done",TRUE,FALSE)</formula>
     </cfRule>
     <cfRule type="expression" dxfId="4" priority="32" stopIfTrue="1">
-      <formula>IF($G12="Cancelled",TRUE,FALSE)</formula>
+      <formula>IF($G13="Cancelled",TRUE,FALSE)</formula>
     </cfRule>
     <cfRule type="expression" dxfId="3" priority="33" stopIfTrue="1">
-      <formula>IF($G12="Pending",TRUE,FALSE)</formula>
+      <formula>IF($G13="Pending",TRUE,FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A18:J19">
+  <conditionalFormatting sqref="A19:J20">
     <cfRule type="expression" dxfId="2" priority="4" stopIfTrue="1">
-      <formula>IF($G18="Done",TRUE,FALSE)</formula>
+      <formula>IF($G19="Done",TRUE,FALSE)</formula>
     </cfRule>
     <cfRule type="expression" dxfId="1" priority="5" stopIfTrue="1">
-      <formula>IF($G18="Cancelled",TRUE,FALSE)</formula>
+      <formula>IF($G19="Cancelled",TRUE,FALSE)</formula>
     </cfRule>
     <cfRule type="expression" dxfId="0" priority="6" stopIfTrue="1">
-      <formula>IF($G18="Pending",TRUE,FALSE)</formula>
+      <formula>IF($G19="Pending",TRUE,FALSE)</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G19 G7:G8 G10:G12" xr:uid="{00000000-0002-0000-0900-000000000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G20 G7:G8 G10:G13" xr:uid="{00000000-0002-0000-0900-000000000000}">
       <formula1>"Pending,Cancelled,Done,In Progress"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>